<commit_message>
Modify temeseries X ticks (former it was dense and hard to read) 	additionally, I added SWoPP paper, and an Excel file for this paper.
</commit_message>
<xml_diff>
--- a/TeX/EuroMPI-USA-2020/Data/Top500-Performance-Share.xlsx
+++ b/TeX/EuroMPI-USA-2020/Data/Top500-Performance-Share.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsushi/AICS/Projects/Survey/Surveys/GIT/MPIsurvey/TeX/EuroMPI-USA-2020/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977CD2F6-A15E-EA41-9364-6597167D954D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0FA812-1726-3649-981E-6294932E5742}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="960" windowWidth="13140" windowHeight="16800" activeTab="1" xr2:uid="{DD1D6BA0-85AC-7144-A62F-D30270C7ACF0}"/>
   </bookViews>
@@ -903,19 +903,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E25FE-23E1-BC41-87F6-E46300DACC03}">
-  <dimension ref="B2:G44"/>
+  <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:8">
       <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
@@ -930,8 +931,12 @@
       <c r="G2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="H2" s="6">
+        <f>G2/$G$44</f>
+        <v>3.5252643948296123E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" s="7" t="s">
         <v>84</v>
       </c>
@@ -944,7 +949,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:8">
       <c r="B4" s="7" t="s">
         <v>71</v>
       </c>
@@ -960,8 +965,12 @@
         <f>SUM(E4:E12)</f>
         <v>126</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="H4" s="6">
+        <f>G4/$G$44</f>
+        <v>0.14806110458284372</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" s="7" t="s">
         <v>79</v>
       </c>
@@ -974,7 +983,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:8">
       <c r="B6" s="7" t="s">
         <v>17</v>
       </c>
@@ -987,7 +996,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:7">
+    <row r="7" spans="2:8">
       <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1000,7 +1009,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="2:8">
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1022,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:8">
       <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
@@ -1026,7 +1035,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="2:8">
       <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:8">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -1053,7 +1062,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:8">
       <c r="B12" s="8" t="s">
         <v>85</v>
       </c>
@@ -1066,7 +1075,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:8">
       <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
@@ -1081,8 +1090,12 @@
       <c r="G13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="H13" s="6">
+        <f>G13/$G$44</f>
+        <v>3.5252643948296123E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
       <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
@@ -1098,8 +1111,12 @@
         <f>SUM(E14:E17)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="2:7">
+      <c r="H14" s="6">
+        <f>G14/$G$44</f>
+        <v>1.2925969447708578E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
       <c r="B15" s="7" t="s">
         <v>69</v>
       </c>
@@ -1112,7 +1129,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:8">
       <c r="B16" s="7" t="s">
         <v>77</v>
       </c>
@@ -1125,7 +1142,7 @@
       </c>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:8">
       <c r="B17" s="7" t="s">
         <v>81</v>
       </c>
@@ -1138,7 +1155,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:8">
       <c r="B18" s="7" t="s">
         <v>10</v>
       </c>
@@ -1156,8 +1173,12 @@
         <f>SUM(E18:E39)</f>
         <v>552</v>
       </c>
-    </row>
-    <row r="19" spans="2:7">
+      <c r="H18" s="6">
+        <f>G18/$G$44</f>
+        <v>0.64864864864864868</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
       <c r="B19" s="7" t="s">
         <v>9</v>
       </c>
@@ -1172,7 +1193,7 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:8">
       <c r="B20" s="7" t="s">
         <v>39</v>
       </c>
@@ -1187,7 +1208,7 @@
       </c>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:8">
       <c r="B21" s="7" t="s">
         <v>15</v>
       </c>
@@ -1202,7 +1223,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:8">
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1215,7 +1236,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:8">
       <c r="B23" s="7" t="s">
         <v>31</v>
       </c>
@@ -1228,7 +1249,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:8">
       <c r="B24" s="7" t="s">
         <v>23</v>
       </c>
@@ -1241,7 +1262,7 @@
       </c>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:8">
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
@@ -1254,7 +1275,7 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:8">
       <c r="B26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1267,7 +1288,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:8">
       <c r="B27" s="7" t="s">
         <v>11</v>
       </c>
@@ -1280,7 +1301,7 @@
       </c>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:8">
       <c r="B28" s="7" t="s">
         <v>64</v>
       </c>
@@ -1293,7 +1314,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:8">
       <c r="B29" s="7" t="s">
         <v>65</v>
       </c>
@@ -1306,7 +1327,7 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:8">
       <c r="B30" s="7" t="s">
         <v>66</v>
       </c>
@@ -1319,7 +1340,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:8">
       <c r="B31" s="7" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1353,7 @@
       </c>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:8">
       <c r="B32" s="7" t="s">
         <v>70</v>
       </c>
@@ -1345,7 +1366,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:8">
       <c r="B33" s="7" t="s">
         <v>73</v>
       </c>
@@ -1358,7 +1379,7 @@
       </c>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:8">
       <c r="B34" s="7" t="s">
         <v>74</v>
       </c>
@@ -1371,7 +1392,7 @@
       </c>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:8">
       <c r="B35" s="7" t="s">
         <v>19</v>
       </c>
@@ -1384,7 +1405,7 @@
       </c>
       <c r="F35" s="7"/>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:8">
       <c r="B36" s="7" t="s">
         <v>78</v>
       </c>
@@ -1397,7 +1418,7 @@
       </c>
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:8">
       <c r="B37" s="7" t="s">
         <v>80</v>
       </c>
@@ -1410,7 +1431,7 @@
       </c>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:8">
       <c r="B38" s="7" t="s">
         <v>82</v>
       </c>
@@ -1423,7 +1444,7 @@
       </c>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:8">
       <c r="B39" s="7" t="s">
         <v>83</v>
       </c>
@@ -1436,7 +1457,7 @@
       </c>
       <c r="F39" s="7"/>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:8">
       <c r="B40" s="7" t="s">
         <v>13</v>
       </c>
@@ -1452,8 +1473,12 @@
         <f>SUM(E40:E41)</f>
         <v>62</v>
       </c>
-    </row>
-    <row r="41" spans="2:7">
+      <c r="H40" s="6">
+        <f>G40/$G$44</f>
+        <v>7.2855464159811992E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
       <c r="B41" s="7" t="s">
         <v>42</v>
       </c>
@@ -1468,7 +1493,7 @@
       </c>
       <c r="F41" s="7"/>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:8">
       <c r="B42" s="7" t="s">
         <v>27</v>
       </c>
@@ -1485,8 +1510,12 @@
       <c r="G42">
         <v>94</v>
       </c>
-    </row>
-    <row r="44" spans="2:7">
+      <c r="H42" s="6">
+        <f>G42/$G$44</f>
+        <v>0.11045828437132785</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
       <c r="E44">
         <f>SUM(E2:E42)</f>
         <v>851</v>

</xml_diff>

<commit_message>
Initial commit of review comments
</commit_message>
<xml_diff>
--- a/TeX/EuroMPI-USA-2020/Data/Top500-Performance-Share.xlsx
+++ b/TeX/EuroMPI-USA-2020/Data/Top500-Performance-Share.xlsx
@@ -1,33 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsushi/AICS/Projects/Survey/Surveys/GIT/MPIsurvey/TeX/EuroMPI-USA-2020/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0FA812-1726-3649-981E-6294932E5742}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43E3B32-C872-A347-833D-5C5D41D4D293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="960" windowWidth="13140" windowHeight="16800" activeTab="1" xr2:uid="{DD1D6BA0-85AC-7144-A62F-D30270C7ACF0}"/>
+    <workbookView xWindow="660" yWindow="960" windowWidth="18660" windowHeight="16200" activeTab="3" xr2:uid="{DD1D6BA0-85AC-7144-A62F-D30270C7ACF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="2" r:id="rId1"/>
     <sheet name="Countries" sheetId="3" r:id="rId2"/>
     <sheet name="Top500" sheetId="1" r:id="rId3"/>
+    <sheet name="Top500 Nov 20" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="90">
   <si>
     <t>Countries</t>
   </si>
@@ -311,13 +321,16 @@
   <si>
     <t xml:space="preserve"> North Amerika</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Morocco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -379,6 +392,13 @@
       <name val="Helvetica"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF3D3C3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -405,7 +425,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -434,6 +454,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -905,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E25FE-23E1-BC41-87F6-E46300DACC03}">
   <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1526,7 +1552,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:E42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E42">
     <sortCondition ref="D2:D42"/>
   </sortState>
   <phoneticPr fontId="5"/>
@@ -1539,12 +1565,13 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2361,22 +2388,23 @@
         <v>6.6076210223845497E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="E34" s="10"/>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:5">
       <c r="A38" s="5" t="s">
         <v>37</v>
       </c>
@@ -2391,4 +2419,1098 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EF0F5C-F79D-4B4D-9F39-998C704B1690}">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <cols>
+    <col min="3" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>113</v>
+      </c>
+      <c r="D2" s="3">
+        <v>22.6</v>
+      </c>
+      <c r="E2" s="4">
+        <v>668704300</v>
+      </c>
+      <c r="F2" s="4">
+        <v>942339598</v>
+      </c>
+      <c r="G2" s="4">
+        <v>15373432</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <f t="shared" ref="I2:I30" si="0">E2/$E$32</f>
+        <v>0.27532724109996437</v>
+      </c>
+      <c r="L2">
+        <f>F2/$F$32</f>
+        <v>0.24501581060004241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="E3" s="4">
+        <v>593700080</v>
+      </c>
+      <c r="F3" s="4">
+        <v>766195745</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10947524</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H29" si="1">H2+1</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="6">
+        <f t="shared" si="0"/>
+        <v>0.2444455719325091</v>
+      </c>
+      <c r="L3">
+        <f>F3/$F$32</f>
+        <v>0.19921700407996479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>214</v>
+      </c>
+      <c r="D4" s="3">
+        <v>42.8</v>
+      </c>
+      <c r="E4" s="4">
+        <v>566635422</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1231757033</v>
+      </c>
+      <c r="G4" s="4">
+        <v>30704256</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.23330217474117343</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L30" si="2">F4/$F$32</f>
+        <v>0.32026665179233843</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>131048770</v>
+      </c>
+      <c r="F5" s="4">
+        <v>197689472</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2664446</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" si="0"/>
+        <v>5.3957027483812765E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>5.1400839285514546E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E6" s="4">
+        <v>89828330</v>
+      </c>
+      <c r="F6" s="4">
+        <v>135469318</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2669472</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6985235883060963E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>3.5223103042312048E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>78529000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>114511528</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1447536</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2332935374184225E-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2.9773910504787525E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>35997040</v>
+      </c>
+      <c r="F8" s="4">
+        <v>76126574</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1084020</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4821148467214973E-2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>1.9793516346337504E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>34067502</v>
+      </c>
+      <c r="F9" s="4">
+        <v>44283532</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1248840</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4026695112963261E-2</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>1.1514071479370135E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>26698060</v>
+      </c>
+      <c r="F10" s="4">
+        <v>47707321</v>
+      </c>
+      <c r="G10" s="4">
+        <v>716096</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0992456908862878E-2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>1.240428392394843E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E11" s="4">
+        <v>26215350</v>
+      </c>
+      <c r="F11" s="4">
+        <v>33955305</v>
+      </c>
+      <c r="G11" s="4">
+        <v>581140</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0793709551396561E-2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>8.8286500921790547E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>24736650</v>
+      </c>
+      <c r="F12" s="4">
+        <v>31795200</v>
+      </c>
+      <c r="G12" s="4">
+        <v>864000</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0184880818854363E-2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>8.2670055654293622E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="E13" s="4">
+        <v>23087540</v>
+      </c>
+      <c r="F13" s="4">
+        <v>29675520</v>
+      </c>
+      <c r="G13" s="4">
+        <v>806400</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="0"/>
+        <v>9.5058887642640727E-3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>7.7158718610674049E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="4">
+        <v>18720660</v>
+      </c>
+      <c r="F14" s="4">
+        <v>31496620</v>
+      </c>
+      <c r="G14" s="4">
+        <v>709220</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="0"/>
+        <v>7.7079026848944432E-3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>8.1893723842659822E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="4">
+        <v>12622710</v>
+      </c>
+      <c r="F15" s="4">
+        <v>21651750</v>
+      </c>
+      <c r="G15" s="4">
+        <v>247952</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="0"/>
+        <v>5.1971789616201535E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>5.6296276718273575E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10991000</v>
+      </c>
+      <c r="F16" s="4">
+        <v>19270566</v>
+      </c>
+      <c r="G16" s="4">
+        <v>214040</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="0"/>
+        <v>4.5253510511742015E-3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>5.0105008419816148E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="2">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="4">
+        <v>10953340</v>
+      </c>
+      <c r="F17" s="4">
+        <v>12082026</v>
+      </c>
+      <c r="G17" s="4">
+        <v>244488</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="0"/>
+        <v>4.5098452081583501E-3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>3.1414231136669139E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="2">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E18" s="4">
+        <v>10913420</v>
+      </c>
+      <c r="F18" s="4">
+        <v>17261875</v>
+      </c>
+      <c r="G18" s="4">
+        <v>261632</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="0"/>
+        <v>4.4934088498685791E-3</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>4.4882251627524272E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="2">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E19" s="4">
+        <v>9147000</v>
+      </c>
+      <c r="F19" s="4">
+        <v>13736550</v>
+      </c>
+      <c r="G19" s="4">
+        <v>163984</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7661164648430914E-3</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>3.5716125484286532E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>9013750</v>
+      </c>
+      <c r="F20" s="4">
+        <v>12164803</v>
+      </c>
+      <c r="G20" s="4">
+        <v>142368</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7112531195998052E-3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>3.1629457938101286E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="4">
+        <v>8023010</v>
+      </c>
+      <c r="F21" s="4">
+        <v>10432510</v>
+      </c>
+      <c r="G21" s="4">
+        <v>287232</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3033333397398897E-3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>2.7125357988437714E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E22" s="4">
+        <v>7095250</v>
+      </c>
+      <c r="F22" s="4">
+        <v>9748685</v>
+      </c>
+      <c r="G22" s="4">
+        <v>209728</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I22" s="6">
+        <f t="shared" si="0"/>
+        <v>2.9213444678231055E-3</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>2.5347358453671545E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="2">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6596440</v>
+      </c>
+      <c r="F23" s="4">
+        <v>8478720</v>
+      </c>
+      <c r="G23" s="4">
+        <v>230400</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I23" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7159682183611634E-3</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>2.2045348174478301E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="2">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>6470800</v>
+      </c>
+      <c r="F24" s="4">
+        <v>10296115</v>
+      </c>
+      <c r="G24" s="4">
+        <v>153216</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I24" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6642381568499703E-3</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>2.6770720110991832E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E25" s="4">
+        <v>5203700</v>
+      </c>
+      <c r="F25" s="4">
+        <v>8228450</v>
+      </c>
+      <c r="G25" s="4">
+        <v>119088</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I25" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1425320048216899E-3</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>2.1394626215547391E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4771700</v>
+      </c>
+      <c r="F26" s="4">
+        <v>6773346</v>
+      </c>
+      <c r="G26" s="4">
+        <v>131968</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9646635984794775E-3</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>1.7611239771594049E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="2">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3158110</v>
+      </c>
+      <c r="F27" s="4">
+        <v>5014730</v>
+      </c>
+      <c r="G27" s="4">
+        <v>71232</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I27" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3002962795217684E-3</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>1.303869792268191E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2">
+        <v>28</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2726078</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3761664</v>
+      </c>
+      <c r="G28" s="4">
+        <v>37920</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I28" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1224146977420494E-3</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>9.7806263911770584E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1649110</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2119680</v>
+      </c>
+      <c r="G29" s="4">
+        <v>57600</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I29" s="6">
+        <f t="shared" si="0"/>
+        <v>6.7899205459029085E-4</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>5.5113370436195752E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1457730</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2011641</v>
+      </c>
+      <c r="G30" s="4">
+        <v>76896</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6">
+        <f t="shared" si="0"/>
+        <v>6.0019470365100245E-4</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>5.2304270275531806E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="10">
+        <f>SUM(E2:E30)</f>
+        <v>2428761852</v>
+      </c>
+      <c r="F32" s="10">
+        <f>SUM(F2:F30)</f>
+        <v>3846035877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I30">
+    <sortCondition descending="1" ref="I2:I30"/>
+  </sortState>
+  <phoneticPr fontId="5"/>
+  <hyperlinks>
+    <hyperlink ref="A31" r:id="rId1" tooltip="TOP500" display="https://www.top500.org/" xr:uid="{D28EB423-C6C0-854A-BED4-8F93D00E132E}"/>
+    <hyperlink ref="A32" r:id="rId2" tooltip="Current List" display="https://www.top500.org/lists/top500/2020/11" xr:uid="{1D1C85C5-DA3F-CC42-B9F4-BDA955F83E93}"/>
+    <hyperlink ref="A34" r:id="rId3" tooltip="25 Year Anniversary" display="https://www.top500.org/25years" xr:uid="{8A69B287-C9A3-4C40-9D4C-C6E9BCD88C0C}"/>
+    <hyperlink ref="A36" r:id="rId4" tooltip="Newsletter" display="https://www.top500.org/accounts/signup" xr:uid="{7BFABC91-C1E5-2049-B42C-737ACC9540CE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>